<commit_message>
Checking list membership: case insensitive by default
</commit_message>
<xml_diff>
--- a/openn/tests/data/sheets/value_lists.xlsx
+++ b/openn/tests/data/sheets/value_lists.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
   <si>
     <t>Note: Please enter one work per page.</t>
   </si>
@@ -155,15 +155,28 @@
   </si>
   <si>
     <t xml:space="preserve">PD </t>
+  </si>
+  <si>
+    <t>Rights PD (lower case)</t>
+  </si>
+  <si>
+    <t>pd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -252,85 +265,88 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="59">
+  <cellStyleXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="15" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="15" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="15" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="15" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="15"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="15" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="15" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="15"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="15" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="15" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="15" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="15" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="15" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="15" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="15" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="15" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="15" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="59">
+  <cellStyles count="61">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -365,6 +381,7 @@
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -388,6 +405,7 @@
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="15"/>
   </cellStyles>
@@ -688,7 +706,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V12"/>
+  <dimension ref="A1:V13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
@@ -895,6 +913,17 @@
       </c>
       <c r="C12" s="10" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22">
+      <c r="A13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>